<commit_message>
red text when manga is not finished. fixed bug when no search result is found.
</commit_message>
<xml_diff>
--- a/scr/Blank.xlsx
+++ b/scr/Blank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/05dc14526b7d9387/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/05dc14526b7d9387/Backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_F7FB4E34AEA0A3236DAA142502A6CE802E7897D8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCAAFFCC-A781-4FE1-A982-0B4414558E58}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{197E366D-0B1C-41CF-B3BE-780E63279D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF939DFC-07CC-43A9-A296-54594640E710}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Manga Liste" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Manga Liste'!$A$4:$G$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Manga Liste'!$B$4:$G$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,10 +70,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="165" formatCode="0.00\€"/>
+    <numFmt numFmtId="164" formatCode="0.00\€"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,8 +166,27 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,22 +260,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -427,6 +461,19 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -442,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -451,12 +498,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -464,9 +505,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -482,16 +520,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -507,12 +536,6 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -531,18 +554,6 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,9 +561,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -583,7 +591,7 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -592,7 +600,7 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -604,13 +612,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -640,12 +645,6 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -658,31 +657,16 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -702,10 +686,10 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -722,6 +706,123 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="19" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,7 +846,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor rgb="FFC6E0B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -760,10 +861,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1068,32 +1165,32 @@
   </sheetPr>
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="99.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" style="45" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="15" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="16" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="94" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" style="95" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="96" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" style="56" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="52" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" style="53" customWidth="1"/>
-    <col min="16" max="40" width="11.42578125" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="13.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="32" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="106" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="112" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="92" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="73" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="74" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="75" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="43" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="39" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="40" customWidth="1"/>
+    <col min="16" max="49" width="11.42578125" style="1" customWidth="1"/>
+    <col min="50" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="60.75" customHeight="1">
+    <row r="1" spans="1:15" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1101,473 +1198,470 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="6"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="1"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-    </row>
-    <row r="2" spans="1:15" ht="18.75" customHeight="1">
+      <c r="H1" s="14"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="6"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="1"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-    </row>
-    <row r="3" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+    </row>
+    <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="87">
         <f>SUM(E5:E840)</f>
         <v>0</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="18">
+      <c r="F3" s="4"/>
+      <c r="G3" s="85">
         <f t="array" ref="G3">SUM(G5:G10000 * E5:E10000)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="85"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-    </row>
-    <row r="4" spans="1:15" ht="30" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="I3" s="64"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+    </row>
+    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="86"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="48"/>
-    </row>
-    <row r="5" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="50"/>
-    </row>
-    <row r="6" spans="1:15" ht="99.95" customHeight="1">
-      <c r="B6" s="40"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="24"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="89"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="50"/>
-    </row>
-    <row r="7" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="92"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="50"/>
-    </row>
-    <row r="8" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="24"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="59"/>
-    </row>
-    <row r="9" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="50"/>
-    </row>
-    <row r="10" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="90"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="50"/>
-    </row>
-    <row r="11" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A11" s="19"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="89"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="50"/>
-    </row>
-    <row r="12" spans="1:15" ht="99.95" customHeight="1">
-      <c r="B12" s="60"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="69"/>
-      <c r="I12" s="93"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="50"/>
-    </row>
-    <row r="13" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="24"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="50"/>
-    </row>
-    <row r="14" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="24"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="50"/>
-    </row>
-    <row r="15" spans="1:15" ht="99.95" customHeight="1">
-      <c r="B15" s="40"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="50"/>
-    </row>
-    <row r="16" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="24"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="50"/>
-    </row>
-    <row r="17" spans="1:15" ht="99.95" customHeight="1">
-      <c r="B17" s="60"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="69"/>
-    </row>
-    <row r="18" spans="1:15" ht="99.95" customHeight="1">
-      <c r="B18" s="43"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="34"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="89"/>
-      <c r="L18" s="90"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="50"/>
-    </row>
-    <row r="19" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="24"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="89"/>
-      <c r="L19" s="90"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="50"/>
-    </row>
-    <row r="20" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="89"/>
-      <c r="L20" s="90"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="50"/>
-    </row>
-    <row r="21" spans="1:15" ht="99.95" customHeight="1">
-      <c r="B21" s="60"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="69"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="97"/>
-      <c r="N21" s="56"/>
-    </row>
-    <row r="22" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="35"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="88"/>
-      <c r="K22" s="89"/>
-      <c r="L22" s="90"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="50"/>
-    </row>
-    <row r="23" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A23" s="11"/>
-      <c r="B23" s="62"/>
-      <c r="F23" s="57"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="89"/>
-      <c r="L23" s="90"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="50"/>
-    </row>
-    <row r="24" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="70"/>
-      <c r="I24" s="93"/>
-      <c r="J24" s="88"/>
-      <c r="K24" s="89"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="50"/>
-    </row>
-    <row r="25" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="70"/>
-    </row>
-    <row r="26" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A26" s="19"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="70"/>
-    </row>
-    <row r="27" spans="1:15" ht="99.95" customHeight="1">
-      <c r="B27" s="79"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="83"/>
-    </row>
-    <row r="28" spans="1:15" ht="99.95" customHeight="1">
-      <c r="B28" s="71"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="75"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="89"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="50"/>
-    </row>
-    <row r="29" spans="1:15" ht="99.95" customHeight="1">
-      <c r="B29" s="44"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="39"/>
-      <c r="J29" s="88"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="89"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="50"/>
-    </row>
-    <row r="30" spans="1:15" ht="99.95" customHeight="1">
-      <c r="B30" s="44"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="39"/>
-      <c r="J30" s="88"/>
-      <c r="K30" s="90"/>
-      <c r="L30" s="89"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="50"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="35"/>
+    </row>
+    <row r="5" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="37"/>
+    </row>
+    <row r="6" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="77"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="108"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="37"/>
+    </row>
+    <row r="7" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="108"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="37"/>
+    </row>
+    <row r="8" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="108"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="45"/>
+    </row>
+    <row r="9" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="108"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="37"/>
+    </row>
+    <row r="10" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="108"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="37"/>
+    </row>
+    <row r="11" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="108"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="37"/>
+    </row>
+    <row r="12" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="81"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="97"/>
+      <c r="G12" s="109"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="37"/>
+    </row>
+    <row r="13" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="110"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="37"/>
+    </row>
+    <row r="14" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="110"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="69"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="37"/>
+    </row>
+    <row r="15" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="27"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="110"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="37"/>
+    </row>
+    <row r="16" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="99"/>
+      <c r="G16" s="110"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="37"/>
+    </row>
+    <row r="17" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="46"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="111"/>
+    </row>
+    <row r="18" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="30"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="101"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="37"/>
+    </row>
+    <row r="19" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="110"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="68"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="37"/>
+    </row>
+    <row r="20" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="110"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="37"/>
+    </row>
+    <row r="21" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="46"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="100"/>
+      <c r="G21" s="111"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="76"/>
+      <c r="N21" s="43"/>
+    </row>
+    <row r="22" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="110"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="68"/>
+      <c r="L22" s="69"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="37"/>
+    </row>
+    <row r="23" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="48"/>
+      <c r="F23" s="11"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="68"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="37"/>
+    </row>
+    <row r="24" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="110"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="37"/>
+    </row>
+    <row r="25" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="110"/>
+    </row>
+    <row r="26" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="110"/>
+    </row>
+    <row r="27" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="59"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="113"/>
+    </row>
+    <row r="28" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="55"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="104"/>
+      <c r="G28" s="114"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="68"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="37"/>
+    </row>
+    <row r="29" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="31"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="105"/>
+      <c r="G29" s="115"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="68"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="37"/>
+    </row>
+    <row r="30" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="31"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="105"/>
+      <c r="G30" s="115"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="37"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:G4" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:G26">
-      <sortCondition ref="B4"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="B4:G4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="E5:E1048576">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>AND($E5 = $F5,NOT(ISBLANK($E5)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>$E5 = INT(LEFT($F5,FIND("/",$F5)-1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>$E5&lt;$F5</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D1:D20 D22:D23 D28:D1048576 L4:L21 L23:L24 L28:L1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"BoysLove,Thriller,Fantasie,Shounen,GirlsLove,Josei,Sience Fiction"</formula1>
-    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A1:H2 A3:G1048576 I1:M1048576 O1:XFD1048576 N1:N4 N6:N1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="47" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293"/>

</xml_diff>

<commit_message>
Added th function to create a list from a preset. fixed bug with the price showing -1
</commit_message>
<xml_diff>
--- a/scr/Blank.xlsx
+++ b/scr/Blank.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/05dc14526b7d9387/Backup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\Projects\MangaListe\scr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{197E366D-0B1C-41CF-B3BE-780E63279D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF939DFC-07CC-43A9-A296-54594640E710}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB387A5E-AEC0-4333-9F00-1EDB98E400EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -498,9 +498,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -758,6 +755,36 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -770,58 +797,31 @@
     <xf numFmtId="49" fontId="10" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1166,26 +1166,26 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" style="32" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="106" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="112" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="92" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="31" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="111" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="98" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="91" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="73" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="74" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="75" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" style="43" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="39" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="40" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="72" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="73" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="74" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="42" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="38" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="39" customWidth="1"/>
     <col min="16" max="49" width="11.42578125" style="1" customWidth="1"/>
     <col min="50" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -1198,16 +1198,16 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="F1" s="102"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1215,437 +1215,436 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="102"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
     </row>
     <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="87">
+      <c r="B3" s="86">
         <f>SUM(E5:E840)</f>
         <v>0</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="85">
+      <c r="F3" s="102"/>
+      <c r="G3" s="84">
         <f t="array" ref="G3">SUM(G5:G10000 * E5:E10000)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="35"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="34"/>
     </row>
     <row r="5" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="37"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="77"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="108"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="37"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="94"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="36"/>
     </row>
     <row r="7" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="108"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="37"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="94"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="36"/>
     </row>
     <row r="8" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="108"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="45"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="94"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="44"/>
     </row>
     <row r="9" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="108"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="37"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="94"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="36"/>
     </row>
     <row r="10" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="108"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="37"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="94"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="36"/>
     </row>
     <row r="11" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="108"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="37"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="94"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="36"/>
     </row>
     <row r="12" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="81"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="109"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="37"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="106"/>
+      <c r="G12" s="95"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="36"/>
     </row>
     <row r="13" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="110"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="37"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="96"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="36"/>
     </row>
     <row r="14" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="99"/>
-      <c r="G14" s="110"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="37"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="96"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="36"/>
     </row>
     <row r="15" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="110"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="37"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="96"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="36"/>
     </row>
     <row r="16" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="110"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="37"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="96"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="36"/>
     </row>
     <row r="17" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="46"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="111"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="97"/>
     </row>
     <row r="18" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="30"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="101"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="37"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="109"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="36"/>
     </row>
     <row r="19" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="110"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="37"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="96"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="36"/>
     </row>
     <row r="20" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="110"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="67"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="37"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="96"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="66"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="36"/>
     </row>
     <row r="21" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="111"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="76"/>
-      <c r="N21" s="43"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="108"/>
+      <c r="G21" s="97"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="75"/>
+      <c r="N21" s="42"/>
     </row>
     <row r="22" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="110"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="69"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="37"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="110"/>
+      <c r="G22" s="96"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="36"/>
     </row>
     <row r="23" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="48"/>
-      <c r="F23" s="11"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="68"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="37"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="47"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="68"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="36"/>
     </row>
     <row r="24" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="110"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="37"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="112"/>
+      <c r="G24" s="96"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="36"/>
     </row>
     <row r="25" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="110"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="96"/>
     </row>
     <row r="26" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="98"/>
-      <c r="G26" s="110"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="107"/>
+      <c r="G26" s="96"/>
     </row>
     <row r="27" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="59"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="103"/>
-      <c r="G27" s="113"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="113"/>
+      <c r="G27" s="99"/>
     </row>
     <row r="28" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="55"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="104"/>
-      <c r="G28" s="114"/>
-      <c r="J28" s="67"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="36"/>
-      <c r="O28" s="37"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="114"/>
+      <c r="G28" s="100"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="68"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="36"/>
     </row>
     <row r="29" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="31"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="115"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="68"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="36"/>
-      <c r="O29" s="37"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="115"/>
+      <c r="G29" s="101"/>
+      <c r="J29" s="66"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="36"/>
     </row>
     <row r="30" spans="1:15" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="31"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="105"/>
-      <c r="G30" s="115"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="68"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="36"/>
-      <c r="O30" s="37"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="115"/>
+      <c r="G30" s="101"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="68"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="36"/>
     </row>
   </sheetData>
   <autoFilter ref="B4:G4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Added the whole template featcher and fixed minor bugs with the update funktion. moved some files around.
</commit_message>
<xml_diff>
--- a/scr/Blank.xlsx
+++ b/scr/Blank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\Projects\MangaListe\scr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB387A5E-AEC0-4333-9F00-1EDB98E400EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B25F2F-0715-4106-8A9B-ECEE98C11572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Manga Liste" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Manga Liste'!$B$4:$G$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Manga Liste'!$A$4:$G$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1166,7 +1166,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1647,7 +1647,7 @@
       <c r="O30" s="36"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:G4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A4:G4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="E5:E1048576">
     <cfRule type="expression" dxfId="2" priority="6">
       <formula>AND($E5 = $F5,NOT(ISBLANK($E5)))</formula>

</xml_diff>